<commit_message>
add planned scrape actions
</commit_message>
<xml_diff>
--- a/Code/Exploratory Data Analysis/All Data/dropout_firms_explanations.xlsx
+++ b/Code/Exploratory Data Analysis/All Data/dropout_firms_explanations.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\Stat-222-Project\Code\Exploratory Data Analysis\All Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7790BC-C9E1-4870-87B9-8EB3744D69A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233F9F73-A9C3-4A63-92D2-6691707C221D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{A098F981-28C5-400F-8F0D-433ADB7BBFEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$35</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>ticker</t>
   </si>
@@ -68,9 +71,6 @@
     <t>CNHI</t>
   </si>
   <si>
-    <t>Earnings call dates or quarters consistently incorrect, check transcripts</t>
-  </si>
-  <si>
     <t>DAR</t>
   </si>
   <si>
@@ -186,6 +186,30 @@
   </si>
   <si>
     <t>XIN</t>
+  </si>
+  <si>
+    <t>potential action</t>
+  </si>
+  <si>
+    <t>no action needed</t>
+  </si>
+  <si>
+    <t>The calls are for Raven Industries, which was acquired by CNHI in 2021. We can drop or try to get correct CNHI calls</t>
+  </si>
+  <si>
+    <t>scrape all calls for this ticker with no date restriction</t>
+  </si>
+  <si>
+    <t>drop company</t>
+  </si>
+  <si>
+    <t>re-scrape all calls from alternative source, drop company if can't find quarterly</t>
+  </si>
+  <si>
+    <t>re-scrape all calls from alternative source, drop company if can't find CNHI</t>
+  </si>
+  <si>
+    <t>add as many calls as possible from alternative source, no action needed on failure</t>
   </si>
 </sst>
 </file>
@@ -557,298 +581,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C6B402-433E-45A3-B228-0A451DC398B1}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="235.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="235.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>38</v>
       </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
         <v>39</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
         <v>41</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>43</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>44</v>
       </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" t="s">
         <v>45</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
         <v>47</v>
       </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" t="s">
-        <v>48</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C35" xr:uid="{74C6B402-433E-45A3-B228-0A451DC398B1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rerun all_data_fixed_quarter after obtaining calls for drop out. Only BTU went bankrupted.
</commit_message>
<xml_diff>
--- a/Code/Exploratory Data Analysis/All Data/dropout_firms_explanations.xlsx
+++ b/Code/Exploratory Data Analysis/All Data/dropout_firms_explanations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15527\OneDrive\Desktop\Code\Stat-222-Project\Code\Exploratory Data Analysis\All Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF46503-209A-419E-AC57-EFB1BE3969BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB6B25C-9641-4745-8355-0968F19B3AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A098F981-28C5-400F-8F0D-433ADB7BBFEF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="104">
   <si>
     <t>ticker</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>Only contributes 3 valid rows after resolving fililng date (1 call per year)</t>
+  </si>
+  <si>
+    <t>latter date have filing date inconsistency</t>
   </si>
 </sst>
 </file>
@@ -363,12 +366,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -383,8 +392,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,7 +733,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F20" sqref="F20"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,110 +767,113 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F5" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
         <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>83</v>
@@ -869,18 +882,18 @@
         <v>86</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
         <v>83</v>
@@ -889,440 +902,437 @@
         <v>86</v>
       </c>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
         <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>92</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F10" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F12" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
         <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
         <v>86</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
         <v>86</v>
       </c>
       <c r="F14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="C26" t="s">
-        <v>81</v>
-      </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
         <v>50</v>
@@ -1336,7 +1346,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
         <v>50</v>
@@ -1350,311 +1360,318 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C56" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="D56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C58" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="D58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B60" t="s">
         <v>50</v>
       </c>
+      <c r="C60" t="s">
+        <v>81</v>
+      </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F61" xr:uid="{74C6B402-433E-45A3-B228-0A451DC398B1}"/>
+  <autoFilter ref="A1:F61" xr:uid="{74C6B402-433E-45A3-B228-0A451DC398B1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
+      <sortCondition ref="F1:F61"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final explanation for drop_out firms
</commit_message>
<xml_diff>
--- a/Code/Exploratory Data Analysis/All Data/dropout_firms_explanations.xlsx
+++ b/Code/Exploratory Data Analysis/All Data/dropout_firms_explanations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15527\OneDrive\Desktop\Code\Stat-222-Project\Code\Exploratory Data Analysis\All Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB6B25C-9641-4745-8355-0968F19B3AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007945B8-225E-4CC7-881A-B08C9CAF160A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A098F981-28C5-400F-8F0D-433ADB7BBFEF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="105">
   <si>
     <t>ticker</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>latter date have filing date inconsistency</t>
+  </si>
+  <si>
+    <t>Dropped out because we manually drop rows with filing date that are not in the fixed quarter .Call is for quarter and year in advance, could pull more calls and financial statement data up to last CALL in 2016. I think financial data already goes past 2016 so would just need to scrape extra calls</t>
   </si>
 </sst>
 </file>
@@ -733,7 +736,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D9" sqref="D9"/>
+      <selection pane="topRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -913,7 +916,7 @@
         <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
Update mindmap, remove BTU after Mar 3, 2015, save to all_data_fixed_quarter_dates.parquet
</commit_message>
<xml_diff>
--- a/Code/Exploratory Data Analysis/All Data/dropout_firms_explanations.xlsx
+++ b/Code/Exploratory Data Analysis/All Data/dropout_firms_explanations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15527\OneDrive\Desktop\Code\Stat-222-Project\Code\Exploratory Data Analysis\All Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007945B8-225E-4CC7-881A-B08C9CAF160A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0EA1D2-5E90-4FDD-B193-0AF1ABCA8C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A098F981-28C5-400F-8F0D-433ADB7BBFEF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="106">
   <si>
     <t>ticker</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>Dropped out because we manually drop rows with filing date that are not in the fixed quarter .Call is for quarter and year in advance, could pull more calls and financial statement data up to last CALL in 2016. I think financial data already goes past 2016 so would just need to scrape extra calls</t>
+  </si>
+  <si>
+    <t>Drop calls after 3/3/2015</t>
   </si>
 </sst>
 </file>
@@ -395,9 +398,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,7 +740,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F20" sqref="F20"/>
+      <selection pane="topRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,262 +774,262 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
         <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
         <v>86</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
         <v>86</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>92</v>
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
         <v>86</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E14" t="s">
         <v>86</v>
       </c>
       <c r="F14" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1672,7 +1676,7 @@
   </sheetData>
   <autoFilter ref="A1:F61" xr:uid="{74C6B402-433E-45A3-B228-0A451DC398B1}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
-      <sortCondition ref="F1:F61"/>
+      <sortCondition ref="E1:E61"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>